<commit_message>
Back to where we left off-run Mill on linux Daycent on Win
</commit_message>
<xml_diff>
--- a/Daycent/Calibration tests_LRF.xlsx
+++ b/Daycent/Calibration tests_LRF.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmaas\Documents\Modeling\Daycent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{674AAE36-0541-41F6-ABDC-13BCD4B3892F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64214734-196A-4756-AE94-BB6F442DF517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="29805" yWindow="690" windowWidth="25860" windowHeight="12765" xr2:uid="{CE6A7311-E17E-48F7-8EE8-BEE5E04D0210}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CE6A7311-E17E-48F7-8EE8-BEE5E04D0210}"/>
   </bookViews>
   <sheets>
     <sheet name="N error-1_3" sheetId="9" r:id="rId1"/>
@@ -241,7 +241,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -254,13 +254,17 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -577,7 +581,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CC3DB169-2D47-490D-93CF-DC312B4081DB}">
   <dimension ref="A1:W35"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F38" sqref="F38"/>
     </sheetView>
   </sheetViews>
@@ -591,36 +595,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="8"/>
+      <c r="O1" s="10"/>
       <c r="P1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="8" t="s">
+      <c r="Q1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1774,8 +1778,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E99348-F096-4696-A2A1-39C427DE3E16}">
   <dimension ref="A1:AC20"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N5" sqref="N5"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1798,41 +1802,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="B1" s="8" t="s">
+      <c r="B1" s="10" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="8"/>
-      <c r="D1" s="8"/>
-      <c r="E1" s="8"/>
-      <c r="F1" s="8"/>
-      <c r="G1" s="8"/>
-      <c r="H1" s="8"/>
-      <c r="I1" s="8"/>
-      <c r="J1" s="8"/>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8" t="s">
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8" t="s">
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8" t="s">
+      <c r="R1" s="10"/>
+      <c r="S1" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="10"/>
+      <c r="AA1" s="10"/>
+      <c r="AB1" s="10"/>
       <c r="AC1" s="7"/>
     </row>
     <row r="2" spans="1:29" ht="58" x14ac:dyDescent="0.35">
@@ -2195,44 +2199,44 @@
         <v>4677</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="A8" s="2">
+    <row r="8" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="11">
         <v>4</v>
       </c>
-      <c r="E8">
+      <c r="E8" s="3">
         <v>3.9</v>
       </c>
-      <c r="K8">
+      <c r="K8" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="S8" s="5" t="s">
+      <c r="S8" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="T8">
+      <c r="T8" s="3">
         <v>1108</v>
       </c>
-      <c r="U8">
+      <c r="U8" s="3">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="V8" s="2">
+      <c r="V8" s="11">
         <v>1108</v>
       </c>
-      <c r="W8" s="2">
-        <v>0</v>
-      </c>
-      <c r="X8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="2">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="2">
+      <c r="W8" s="11">
+        <v>0</v>
+      </c>
+      <c r="X8" s="11">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="11">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="11">
         <v>5889</v>
       </c>
-      <c r="AA8" s="2">
+      <c r="AA8" s="11">
         <v>1138</v>
       </c>
-      <c r="AB8" s="2">
+      <c r="AB8" s="11">
         <v>4740</v>
       </c>
     </row>
@@ -2634,86 +2638,86 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="20" spans="1:28" s="10" customFormat="1" ht="29" x14ac:dyDescent="0.35">
-      <c r="A20" s="9" t="s">
+    <row r="20" spans="1:28" s="9" customFormat="1" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="B20" s="10">
+      <c r="B20" s="9">
         <v>0.2</v>
       </c>
-      <c r="C20" s="10">
+      <c r="C20" s="9">
         <v>0.7</v>
       </c>
-      <c r="D20" s="10">
+      <c r="D20" s="9">
         <v>0.8</v>
       </c>
-      <c r="E20" s="10">
+      <c r="E20" s="9">
         <v>3.9</v>
       </c>
-      <c r="F20" s="10">
+      <c r="F20" s="9">
         <v>7</v>
       </c>
-      <c r="G20" s="10">
+      <c r="G20" s="9">
         <v>10</v>
       </c>
-      <c r="H20" s="10">
+      <c r="H20" s="9">
         <v>10</v>
       </c>
-      <c r="I20" s="10">
+      <c r="I20" s="9">
         <v>9</v>
       </c>
-      <c r="J20" s="10">
+      <c r="J20" s="9">
         <v>5</v>
       </c>
-      <c r="K20" s="10">
+      <c r="K20" s="9">
         <v>8.5000000000000006E-3</v>
       </c>
-      <c r="L20" s="10">
+      <c r="L20" s="9">
         <v>0.5</v>
       </c>
-      <c r="M20" s="10">
+      <c r="M20" s="9">
         <v>0.05</v>
       </c>
-      <c r="N20" s="10">
+      <c r="N20" s="9">
         <v>0.2</v>
       </c>
-      <c r="O20" s="10">
+      <c r="O20" s="9">
         <v>0.1</v>
       </c>
-      <c r="P20" s="10">
+      <c r="P20" s="9">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="Q20" s="9" t="s">
+      <c r="Q20" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="R20" s="10" t="s">
+      <c r="R20" s="9" t="s">
         <v>51</v>
       </c>
-      <c r="T20" s="10">
+      <c r="T20" s="9">
         <v>1958</v>
       </c>
-      <c r="U20" s="10">
+      <c r="U20" s="9">
         <v>8.5000000000000006E-2</v>
       </c>
-      <c r="V20" s="9">
+      <c r="V20" s="8">
         <v>1958</v>
       </c>
-      <c r="W20" s="9">
-        <v>0</v>
-      </c>
-      <c r="X20" s="9">
-        <v>0</v>
-      </c>
-      <c r="Y20" s="9">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="9">
+      <c r="W20" s="8">
+        <v>0</v>
+      </c>
+      <c r="X20" s="8">
+        <v>0</v>
+      </c>
+      <c r="Y20" s="8">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="8">
         <v>3649</v>
       </c>
-      <c r="AA20" s="9">
+      <c r="AA20" s="8">
         <v>673</v>
       </c>
-      <c r="AB20" s="9">
+      <c r="AB20" s="8">
         <v>2969</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Pub changes; Daycent rerun files
</commit_message>
<xml_diff>
--- a/Daycent/Calibration tests_LRF.xlsx
+++ b/Daycent/Calibration tests_LRF.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\edmaas\Documents\Modeling\Daycent\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64214734-196A-4756-AE94-BB6F442DF517}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F083C53-D34C-4B48-8CF0-0C9BDF93F71E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{CE6A7311-E17E-48F7-8EE8-BEE5E04D0210}"/>
   </bookViews>
@@ -200,8 +200,16 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <strike/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -241,7 +249,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -258,13 +266,14 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -595,36 +604,36 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23" x14ac:dyDescent="0.35">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="10"/>
+      <c r="O1" s="12"/>
       <c r="P1" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="Q1" s="10" t="s">
+      <c r="Q1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
@@ -1776,10 +1785,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58E99348-F096-4696-A2A1-39C427DE3E16}">
-  <dimension ref="A1:AC20"/>
+  <dimension ref="A1:AC21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1802,41 +1811,41 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.35">
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10" t="s">
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10" t="s">
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12" t="s">
         <v>8</v>
       </c>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10" t="s">
+      <c r="R1" s="12"/>
+      <c r="S1" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="12"/>
+      <c r="X1" s="12"/>
+      <c r="Y1" s="12"/>
+      <c r="Z1" s="12"/>
+      <c r="AA1" s="12"/>
+      <c r="AB1" s="12"/>
       <c r="AC1" s="7"/>
     </row>
     <row r="2" spans="1:29" ht="58" x14ac:dyDescent="0.35">
@@ -1925,7 +1934,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="3" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:29" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>33</v>
       </c>
@@ -2011,7 +2020,7 @@
         <v>3270</v>
       </c>
     </row>
-    <row r="4" spans="1:29" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:29" ht="43.5" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>48</v>
       </c>
@@ -2085,7 +2094,7 @@
         <v>5287</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>1</v>
       </c>
@@ -2123,7 +2132,7 @@
         <v>4673</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>2</v>
       </c>
@@ -2161,7 +2170,7 @@
         <v>4677</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -2199,8 +2208,8 @@
         <v>4677</v>
       </c>
     </row>
-    <row r="8" spans="1:29" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A8" s="11">
+    <row r="8" spans="1:29" s="3" customFormat="1" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A8" s="10">
         <v>4</v>
       </c>
       <c r="E8" s="3">
@@ -2209,7 +2218,7 @@
       <c r="K8" s="3">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="S8" s="12" t="s">
+      <c r="S8" s="11" t="s">
         <v>32</v>
       </c>
       <c r="T8" s="3">
@@ -2218,29 +2227,29 @@
       <c r="U8" s="3">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="V8" s="11">
+      <c r="V8" s="10">
         <v>1108</v>
       </c>
-      <c r="W8" s="11">
-        <v>0</v>
-      </c>
-      <c r="X8" s="11">
-        <v>0</v>
-      </c>
-      <c r="Y8" s="11">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="11">
+      <c r="W8" s="10">
+        <v>0</v>
+      </c>
+      <c r="X8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Y8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="10">
         <v>5889</v>
       </c>
-      <c r="AA8" s="11">
+      <c r="AA8" s="10">
         <v>1138</v>
       </c>
-      <c r="AB8" s="11">
+      <c r="AB8" s="10">
         <v>4740</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>5</v>
       </c>
@@ -2281,7 +2290,7 @@
         <v>4741</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>6</v>
       </c>
@@ -2325,7 +2334,7 @@
         <v>3448</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>7</v>
       </c>
@@ -2366,7 +2375,7 @@
         <v>3489</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>8</v>
       </c>
@@ -2407,7 +2416,7 @@
         <v>3505</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:29" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>9</v>
       </c>
@@ -2669,7 +2678,7 @@
       <c r="J20" s="9">
         <v>5</v>
       </c>
-      <c r="K20" s="9">
+      <c r="K20" s="13">
         <v>8.5000000000000006E-3</v>
       </c>
       <c r="L20" s="9">
@@ -2719,6 +2728,11 @@
       </c>
       <c r="AB20" s="8">
         <v>2969</v>
+      </c>
+    </row>
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
+      <c r="K21" s="9">
+        <v>8.9999999999999993E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>